<commit_message>
Fix layout, import file, filter chuyên ngành theo khoa, toast thông báo hiện
</commit_message>
<xml_diff>
--- a/DuLieuMySQL.xlsx
+++ b/DuLieuMySQL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TanCB\Nam IV\HKI\Cong nghe moi\Lam de tai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7395E2-25D0-48DC-A7B4-5B2C2B8ACEC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C602AC0-037E-47E4-817C-1937FB7F5904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{591E39AF-5A10-4939-8527-1B28A00EF698}"/>
+    <workbookView xWindow="3408" yWindow="2040" windowWidth="17280" windowHeight="8964" firstSheet="1" activeTab="7" xr2:uid="{591E39AF-5A10-4939-8527-1B28A00EF698}"/>
   </bookViews>
   <sheets>
     <sheet name="LopHoc" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="170">
   <si>
     <t xml:space="preserve">Mã lớp </t>
   </si>
@@ -406,9 +406,6 @@
     <t>Role_name</t>
   </si>
   <si>
-    <t>USER</t>
-  </si>
-  <si>
     <t>Mã lịch học</t>
   </si>
   <si>
@@ -533,6 +530,30 @@
   </si>
   <si>
     <t>K18</t>
+  </si>
+  <si>
+    <t>ROLE_USER</t>
+  </si>
+  <si>
+    <t>$2a$10$XLoH1JMRgNOhmm/mHsn3ae2UXdQtMAfxvVItnBFEpm8sBaxj1SySO</t>
+  </si>
+  <si>
+    <t>422000006</t>
+  </si>
+  <si>
+    <t>422000005</t>
+  </si>
+  <si>
+    <t>422000004</t>
+  </si>
+  <si>
+    <t>422000003</t>
+  </si>
+  <si>
+    <t>422000002</t>
+  </si>
+  <si>
+    <t>422000001</t>
   </si>
 </sst>
 </file>
@@ -608,11 +629,11 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1003,16 +1024,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" t="s">
         <v>121</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>122</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>123</v>
-      </c>
-      <c r="D1" t="s">
-        <v>124</v>
       </c>
       <c r="E1" t="s">
         <v>100</v>
@@ -1026,16 +1047,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>130</v>
       </c>
       <c r="E2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1046,16 +1067,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C3" t="s">
-        <v>126</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>132</v>
+        <v>125</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>131</v>
       </c>
       <c r="E3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -1066,16 +1087,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>132</v>
+        <v>126</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>131</v>
       </c>
       <c r="E4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -1086,16 +1107,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>133</v>
+        <v>127</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>132</v>
       </c>
       <c r="E5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -1106,16 +1127,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C6" t="s">
-        <v>129</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>134</v>
+        <v>128</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>133</v>
       </c>
       <c r="E6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F6">
         <v>5</v>
@@ -1126,16 +1147,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>135</v>
+        <v>129</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>134</v>
       </c>
       <c r="E7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F7">
         <v>6</v>
@@ -1165,7 +1186,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B1" t="s">
         <v>26</v>
@@ -1180,7 +1201,7 @@
         <v>100</v>
       </c>
       <c r="F1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1188,16 +1209,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="9">
         <v>33003</v>
       </c>
       <c r="E2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1208,16 +1229,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="9">
         <v>34732</v>
       </c>
       <c r="E3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F3">
         <v>3</v>
@@ -1228,16 +1249,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <v>32579</v>
       </c>
       <c r="E4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F4">
         <v>5</v>
@@ -1248,16 +1269,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C5" t="b">
         <v>1</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <v>31413</v>
       </c>
       <c r="E5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F5">
         <v>7</v>
@@ -1268,16 +1289,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C6" t="b">
         <v>1</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>35099</v>
       </c>
       <c r="E6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F6">
         <v>2</v>
@@ -1288,16 +1309,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C7" t="b">
         <v>0</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <v>33338</v>
       </c>
       <c r="E7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F7">
         <v>4</v>
@@ -1321,8 +1342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4171BD7-A20B-4AA4-8726-87E3F2B67B9E}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1412,11 +1433,11 @@
       <c r="G2" s="7">
         <v>43781</v>
       </c>
-      <c r="H2" s="8">
-        <v>1111</v>
+      <c r="H2" s="10" t="s">
+        <v>163</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>120</v>
+        <v>162</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>61</v>
@@ -1459,11 +1480,11 @@
       <c r="G3" s="7">
         <v>43564</v>
       </c>
-      <c r="H3" s="8">
-        <v>1111</v>
+      <c r="H3" s="10" t="s">
+        <v>163</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>120</v>
+        <v>162</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>62</v>
@@ -1506,11 +1527,11 @@
       <c r="G4" s="7">
         <v>43831</v>
       </c>
-      <c r="H4" s="8">
-        <v>1111</v>
+      <c r="H4" s="10" t="s">
+        <v>163</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>120</v>
+        <v>162</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>63</v>
@@ -1553,11 +1574,11 @@
       <c r="G5" s="7">
         <v>43681</v>
       </c>
-      <c r="H5" s="8">
-        <v>1111</v>
+      <c r="H5" s="10" t="s">
+        <v>163</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>120</v>
+        <v>162</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>64</v>
@@ -1600,11 +1621,11 @@
       <c r="G6" s="7">
         <v>44261</v>
       </c>
-      <c r="H6" s="8">
-        <v>1111</v>
+      <c r="H6" s="10" t="s">
+        <v>163</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>120</v>
+        <v>162</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>65</v>
@@ -1645,7 +1666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B24269-E934-4255-BB25-5BCEE7EFBD5D}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -1680,7 +1701,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C2">
         <v>2022</v>
@@ -1697,7 +1718,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C3">
         <v>2022</v>
@@ -1714,7 +1735,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C4">
         <v>2022</v>
@@ -1731,7 +1752,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C5">
         <v>2023</v>
@@ -1748,7 +1769,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C6">
         <v>2023</v>
@@ -1765,7 +1786,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C7">
         <v>2023</v>
@@ -1782,7 +1803,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C8">
         <v>2024</v>
@@ -1799,7 +1820,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C9">
         <v>2024</v>
@@ -1816,7 +1837,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C10">
         <v>2024</v>
@@ -2256,7 +2277,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C2" t="s">
         <v>45</v>
@@ -2267,7 +2288,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C3" t="s">
         <v>40</v>
@@ -2278,7 +2299,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C4" t="s">
         <v>46</v>
@@ -2289,7 +2310,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C5" t="s">
         <v>47</v>
@@ -2300,7 +2321,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C6" t="s">
         <v>48</v>
@@ -2311,7 +2332,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C7" t="s">
         <v>49</v>
@@ -2326,8 +2347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D4BB23E-9A23-4DB4-B14F-8196D9B0CBF9}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2381,7 +2402,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C2">
         <v>30</v>
@@ -2404,8 +2425,8 @@
       <c r="I2">
         <v>7</v>
       </c>
-      <c r="J2">
-        <v>1</v>
+      <c r="J2" s="1" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -2413,7 +2434,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -2436,8 +2457,8 @@
       <c r="I3">
         <v>2</v>
       </c>
-      <c r="J3">
-        <v>2</v>
+      <c r="J3" s="1" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -2445,7 +2466,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C4">
         <v>60</v>
@@ -2468,8 +2489,8 @@
       <c r="I4">
         <v>4</v>
       </c>
-      <c r="J4">
-        <v>3</v>
+      <c r="J4" s="1" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -2477,7 +2498,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -2500,8 +2521,8 @@
       <c r="I5">
         <v>6</v>
       </c>
-      <c r="J5">
-        <v>4</v>
+      <c r="J5" s="1" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -2509,7 +2530,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C6">
         <v>60</v>
@@ -2532,8 +2553,8 @@
       <c r="I6">
         <v>5</v>
       </c>
-      <c r="J6">
-        <v>5</v>
+      <c r="J6" s="1" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -2541,7 +2562,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C7">
         <v>20</v>
@@ -2564,8 +2585,8 @@
       <c r="I7">
         <v>8</v>
       </c>
-      <c r="J7">
-        <v>6</v>
+      <c r="J7" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2604,10 +2625,10 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" t="s">
         <v>149</v>
-      </c>
-      <c r="E1" t="s">
-        <v>150</v>
       </c>
       <c r="F1" t="s">
         <v>99</v>
@@ -2627,7 +2648,7 @@
         <v>102</v>
       </c>
       <c r="C2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>101</v>
@@ -2653,7 +2674,7 @@
         <v>103</v>
       </c>
       <c r="C3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>114</v>
@@ -2679,7 +2700,7 @@
         <v>104</v>
       </c>
       <c r="C4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>115</v>
@@ -2705,7 +2726,7 @@
         <v>105</v>
       </c>
       <c r="C5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>116</v>
@@ -2731,7 +2752,7 @@
         <v>106</v>
       </c>
       <c r="C6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>117</v>
@@ -2757,7 +2778,7 @@
         <v>107</v>
       </c>
       <c r="C7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>118</v>

</xml_diff>

<commit_message>
Sửa lại kết quả học tập và sinh viên
</commit_message>
<xml_diff>
--- a/DuLieuMySQL.xlsx
+++ b/DuLieuMySQL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TanCB\Nam IV\HKI\Cong nghe moi\Lam de tai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C602AC0-037E-47E4-817C-1937FB7F5904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F0C8B6-1A0F-441D-B6B6-B04D43AAE2F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3408" yWindow="2040" windowWidth="17280" windowHeight="8964" firstSheet="1" activeTab="7" xr2:uid="{591E39AF-5A10-4939-8527-1B28A00EF698}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="6" xr2:uid="{591E39AF-5A10-4939-8527-1B28A00EF698}"/>
   </bookViews>
   <sheets>
     <sheet name="LopHoc" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,12 @@
     <sheet name="Khoa" sheetId="2" r:id="rId4"/>
     <sheet name="ChuyenNganh" sheetId="5" r:id="rId5"/>
     <sheet name="HocPhan" sheetId="6" r:id="rId6"/>
-    <sheet name="MonHoc" sheetId="7" r:id="rId7"/>
-    <sheet name="LopHocPhan" sheetId="9" r:id="rId8"/>
-    <sheet name="ChiTietLopHocPhan" sheetId="10" r:id="rId9"/>
-    <sheet name="LichHoc" sheetId="13" r:id="rId10"/>
-    <sheet name="GiangVien" sheetId="14" r:id="rId11"/>
+    <sheet name="KetQuaHocTap" sheetId="15" r:id="rId7"/>
+    <sheet name="MonHoc" sheetId="7" r:id="rId8"/>
+    <sheet name="LopHocPhan" sheetId="9" r:id="rId9"/>
+    <sheet name="ChiTietLopHocPhan" sheetId="10" r:id="rId10"/>
+    <sheet name="LichHoc" sheetId="13" r:id="rId11"/>
+    <sheet name="GiangVien" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="183">
   <si>
     <t xml:space="preserve">Mã lớp </t>
   </si>
@@ -554,6 +555,45 @@
   </si>
   <si>
     <t>422000001</t>
+  </si>
+  <si>
+    <t>Điểm CK</t>
+  </si>
+  <si>
+    <t>Điểm GK</t>
+  </si>
+  <si>
+    <t>TH1</t>
+  </si>
+  <si>
+    <t>TH2</t>
+  </si>
+  <si>
+    <t>TK1</t>
+  </si>
+  <si>
+    <t>TK2</t>
+  </si>
+  <si>
+    <t>TK3</t>
+  </si>
+  <si>
+    <t>mã lớp hp</t>
+  </si>
+  <si>
+    <t>mã sinh viên</t>
+  </si>
+  <si>
+    <t>18000002</t>
+  </si>
+  <si>
+    <t>18000003</t>
+  </si>
+  <si>
+    <t>18000004</t>
+  </si>
+  <si>
+    <t>18000001</t>
   </si>
 </sst>
 </file>
@@ -614,7 +654,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -634,6 +674,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1007,6 +1051,213 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5CB79E-54E6-42A9-BCAF-3EE0A7DB28E3}">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.88671875" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" customWidth="1"/>
+    <col min="7" max="7" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G2" s="6">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G3" s="6">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4" s="6">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G4" s="6">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" t="s">
+        <v>157</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E5" s="6">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>111</v>
+      </c>
+      <c r="G5" s="6">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" s="6">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G6" s="6">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" t="s">
+        <v>157</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E7" s="6">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G7" s="6">
+        <v>6</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2DA8FC9-C658-4836-AC4C-E4617BF101FC}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -1167,7 +1418,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C70586-B43C-42C5-AD70-272C21ED71BB}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -2248,6 +2499,324 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{054A55DA-B728-455A-B325-491EEA2BB41E}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="7.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="4.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="4.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.21875" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.88671875" customWidth="1"/>
+    <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="H1" t="s">
+        <v>177</v>
+      </c>
+      <c r="I1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="12">
+        <v>8</v>
+      </c>
+      <c r="B2" s="12">
+        <v>8.5</v>
+      </c>
+      <c r="C2" s="12">
+        <v>8</v>
+      </c>
+      <c r="D2" s="12">
+        <v>8</v>
+      </c>
+      <c r="E2" s="12">
+        <v>8</v>
+      </c>
+      <c r="F2" s="12">
+        <v>8</v>
+      </c>
+      <c r="G2" s="12">
+        <v>8</v>
+      </c>
+      <c r="H2" s="11">
+        <v>420000012</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" s="12">
+        <v>4</v>
+      </c>
+      <c r="C3" s="12">
+        <v>4</v>
+      </c>
+      <c r="D3" s="12">
+        <v>4</v>
+      </c>
+      <c r="E3" s="12">
+        <v>4</v>
+      </c>
+      <c r="F3" s="12">
+        <v>4</v>
+      </c>
+      <c r="G3" s="12">
+        <v>4</v>
+      </c>
+      <c r="H3" s="11">
+        <v>420000013</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4" s="11">
+        <v>420000013</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="12">
+        <v>8</v>
+      </c>
+      <c r="B5" s="12">
+        <v>8.5</v>
+      </c>
+      <c r="C5" s="12">
+        <v>8</v>
+      </c>
+      <c r="D5" s="12">
+        <v>8</v>
+      </c>
+      <c r="E5" s="12">
+        <v>8</v>
+      </c>
+      <c r="F5" s="12">
+        <v>8</v>
+      </c>
+      <c r="G5" s="12">
+        <v>8</v>
+      </c>
+      <c r="H5" s="11">
+        <v>420000012</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="12">
+        <v>4</v>
+      </c>
+      <c r="C6" s="12">
+        <v>4</v>
+      </c>
+      <c r="D6" s="12">
+        <v>4</v>
+      </c>
+      <c r="E6" s="12">
+        <v>4</v>
+      </c>
+      <c r="F6" s="12">
+        <v>4</v>
+      </c>
+      <c r="G6" s="12">
+        <v>4</v>
+      </c>
+      <c r="H6" s="11">
+        <v>420000013</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>10</v>
+      </c>
+      <c r="H7" s="11">
+        <v>420000011</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="12">
+        <v>8</v>
+      </c>
+      <c r="B8" s="12">
+        <v>8.5</v>
+      </c>
+      <c r="C8" s="12">
+        <v>8</v>
+      </c>
+      <c r="D8" s="12">
+        <v>8</v>
+      </c>
+      <c r="E8" s="12">
+        <v>8</v>
+      </c>
+      <c r="F8" s="12">
+        <v>8</v>
+      </c>
+      <c r="G8" s="12">
+        <v>8</v>
+      </c>
+      <c r="H8" s="11">
+        <v>420000008</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" s="12">
+        <v>4</v>
+      </c>
+      <c r="C9" s="12">
+        <v>4</v>
+      </c>
+      <c r="D9" s="12">
+        <v>4</v>
+      </c>
+      <c r="E9" s="12">
+        <v>4</v>
+      </c>
+      <c r="F9" s="12">
+        <v>4</v>
+      </c>
+      <c r="G9" s="12">
+        <v>4</v>
+      </c>
+      <c r="H9" s="11">
+        <v>420000009</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+      <c r="F10">
+        <v>10</v>
+      </c>
+      <c r="G10">
+        <v>10</v>
+      </c>
+      <c r="H10" s="11">
+        <v>420000010</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DCB3DAC-2A1A-443C-BFE6-6E88C506D4A4}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -2343,11 +2912,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D4BB23E-9A23-4DB4-B14F-8196D9B0CBF9}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D7" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -2592,211 +3161,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5CB79E-54E6-42A9-BCAF-3EE0A7DB28E3}">
-  <dimension ref="A1:H7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" customWidth="1"/>
-    <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.88671875" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" customWidth="1"/>
-    <col min="7" max="7" width="29.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E1" t="s">
-        <v>149</v>
-      </c>
-      <c r="F1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2" t="s">
-        <v>157</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="E2" s="6">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G2" s="6">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C3" t="s">
-        <v>157</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="E3" s="6">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>109</v>
-      </c>
-      <c r="G3" s="6">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>104</v>
-      </c>
-      <c r="C4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E4" s="6">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>110</v>
-      </c>
-      <c r="G4" s="6">
-        <v>3</v>
-      </c>
-      <c r="H4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C5" t="s">
-        <v>157</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="E5" s="6">
-        <v>2</v>
-      </c>
-      <c r="F5" t="s">
-        <v>111</v>
-      </c>
-      <c r="G5" s="6">
-        <v>4</v>
-      </c>
-      <c r="H5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>106</v>
-      </c>
-      <c r="C6" t="s">
-        <v>157</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="E6" s="6">
-        <v>2</v>
-      </c>
-      <c r="F6" t="s">
-        <v>112</v>
-      </c>
-      <c r="G6" s="6">
-        <v>5</v>
-      </c>
-      <c r="H6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>107</v>
-      </c>
-      <c r="C7" t="s">
-        <v>157</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="E7" s="6">
-        <v>2</v>
-      </c>
-      <c r="F7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G7" s="6">
-        <v>6</v>
-      </c>
-      <c r="H7">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>